<commit_message>
TAB-8861 - Support online event fields in SGT spreadsheet imports
</commit_message>
<xml_diff>
--- a/common/src/test/resources/sgt-import.xlsx
+++ b/common/src/test/resources/sgt-import.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="88">
   <si>
     <t xml:space="preserve">Module</t>
   </si>
@@ -150,6 +150,15 @@
     <t xml:space="preserve">Link text</t>
   </si>
   <si>
+    <t xml:space="preserve">Delivery Method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online Delivery URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online Platform</t>
+  </si>
+  <si>
     <t xml:space="preserve">u0000001,u0000002</t>
   </si>
   <si>
@@ -174,12 +183,30 @@
     <t xml:space="preserve">cuscav</t>
   </si>
   <si>
+    <t xml:space="preserve">Hybrid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tabula.warwick.ac.uk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teams</t>
+  </si>
+  <si>
     <t xml:space="preserve">curef</t>
   </si>
   <si>
+    <t xml:space="preserve">OnlineOnly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moodle</t>
+  </si>
+  <si>
     <t xml:space="preserve">S0.28</t>
   </si>
   <si>
+    <t xml:space="preserve">FaceToFaceOnly</t>
+  </si>
+  <si>
     <t xml:space="preserve">u1234567</t>
   </si>
   <si>
@@ -193,6 +220,9 @@
   </si>
   <si>
     <t xml:space="preserve">S0.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Junk</t>
   </si>
   <si>
     <t xml:space="preserve">u1784383</t>
@@ -684,10 +714,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -703,10 +733,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="8.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="19.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="2" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="10.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="16.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="24.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="20.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="2" width="8.83"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -746,6 +782,16 @@
       <c r="M1" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -758,13 +804,13 @@
         <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H2" s="3" t="n">
         <v>0.458333333333333</v>
@@ -773,13 +819,13 @@
         <v>0.5</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -793,16 +839,16 @@
         <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>7</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H3" s="3" t="n">
         <v>0.458333333333333</v>
@@ -811,7 +857,16 @@
         <v>0.5</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -825,13 +880,13 @@
         <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H4" s="3" t="n">
         <v>0.458333333333333</v>
@@ -839,11 +894,17 @@
       <c r="I4" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -854,16 +915,16 @@
         <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>7</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H5" s="3" t="n">
         <v>0.458333333333333</v>
@@ -872,7 +933,10 @@
         <v>0.5</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -886,13 +950,13 @@
         <v>22</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H6" s="3" t="n">
         <v>0.458333333333333</v>
@@ -901,7 +965,7 @@
         <v>0.5</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -915,16 +979,16 @@
         <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>7</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H7" s="3" t="n">
         <v>0.458333333333333</v>
@@ -933,7 +997,7 @@
         <v>0.5</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -947,13 +1011,13 @@
         <v>23</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H8" s="3" t="n">
         <v>0.458333333333333</v>
@@ -962,7 +1026,10 @@
         <v>0.5</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>54</v>
+        <v>63</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -976,16 +1043,16 @@
         <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>7</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H9" s="3" t="n">
         <v>0.458333333333333</v>
@@ -994,7 +1061,10 @@
         <v>0.5</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>54</v>
+        <v>63</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1008,10 +1078,10 @@
         <v>24</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H10" s="3" t="n">
         <v>0.458333333333333</v>
@@ -1020,7 +1090,7 @@
         <v>0.5</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1034,13 +1104,13 @@
         <v>24</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>7</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H11" s="3" t="n">
         <v>0.458333333333333</v>
@@ -1049,7 +1119,7 @@
         <v>0.5</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1063,10 +1133,10 @@
         <v>25</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H12" s="3" t="n">
         <v>0.458333333333333</v>
@@ -1075,7 +1145,7 @@
         <v>0.5</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1089,13 +1159,13 @@
         <v>25</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>7</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H13" s="3" t="n">
         <v>0.458333333333333</v>
@@ -1104,7 +1174,7 @@
         <v>0.5</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1118,13 +1188,13 @@
         <v>26</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H14" s="3" t="n">
         <v>0.583333333333333</v>
@@ -1133,7 +1203,7 @@
         <v>0.666666666666667</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1147,13 +1217,13 @@
         <v>27</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="H15" s="3" t="n">
         <v>0.583333333333333</v>
@@ -1162,7 +1232,7 @@
         <v>0.666666666666667</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1176,13 +1246,13 @@
         <v>28</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="H16" s="3" t="n">
         <v>0.583333333333333</v>
@@ -1191,7 +1261,7 @@
         <v>0.666666666666667</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1205,13 +1275,13 @@
         <v>29</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="H17" s="3" t="n">
         <v>0.583333333333333</v>
@@ -1220,10 +1290,10 @@
         <v>0.666666666666667</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1235,6 +1305,8 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" display="https://warwick.ac.uk"/>
+    <hyperlink ref="O3" r:id="rId2" display="https://tabula.warwick.ac.uk"/>
+    <hyperlink ref="O4" r:id="rId3" display="https://tabula.warwick.ac.uk"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1269,13 +1341,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,7 +1358,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1294,63 +1366,63 @@
         <v>14</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>